<commit_message>
tree and graph correct result
</commit_message>
<xml_diff>
--- a/CoPilot_on_Algorithm_Design/Sorting_Algorithms/Bubble_Sort/simiparity_comparison.xlsx
+++ b/CoPilot_on_Algorithm_Design/Sorting_Algorithms/Bubble_Sort/simiparity_comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GH-Dataset\Copilot_asset_liability\CopilotEvaluation\CoPilot_on_Algorithm_Design\Sorting_Algorithms\Bubble_Sort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DB6A08E-ADCE-4D81-AB78-03FCFDFE4E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95A846D-AF0D-4E49-B7B8-B3DE540C6420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simiparity_comparison" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,20 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet1!$A$1:$H$145</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet2!$A$1:$H$119</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -117,7 +130,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -944,14 +957,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2561,7 +2574,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2641,7 +2654,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H145"/>
   <sheetViews>
@@ -6557,7 +6570,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H145">
+  <autoFilter ref="A1:H145" xr:uid="{00000000-0009-0000-0000-000002000000}">
     <filterColumn colId="7">
       <filters>
         <filter val="FALSE"/>
@@ -6569,15 +6582,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M90" sqref="M90"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -6596,7 +6612,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -6622,7 +6638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -6648,7 +6664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -6674,7 +6690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -6700,7 +6716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -6726,7 +6742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -6752,7 +6768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -6778,7 +6794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -6804,7 +6820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -6830,7 +6846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -6856,7 +6872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -6882,7 +6898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -6908,7 +6924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -6934,7 +6950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -6960,7 +6976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -6986,7 +7002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -7012,7 +7028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -7038,7 +7054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -7064,7 +7080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -7090,7 +7106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -7116,7 +7132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -7142,7 +7158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -7168,7 +7184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -7194,7 +7210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -7220,7 +7236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -7246,7 +7262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -7272,7 +7288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -7298,7 +7314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -7324,7 +7340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -7350,7 +7366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -7376,7 +7392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -7402,7 +7418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -7428,7 +7444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -7454,7 +7470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -7480,7 +7496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -7506,7 +7522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -7532,7 +7548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -7558,7 +7574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -7584,7 +7600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -7610,7 +7626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -7636,7 +7652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>16</v>
       </c>
@@ -7662,7 +7678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -7688,7 +7704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>16</v>
       </c>
@@ -7714,7 +7730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>16</v>
       </c>
@@ -7740,7 +7756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -7766,7 +7782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>16</v>
       </c>
@@ -7792,7 +7808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -7818,7 +7834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -7844,7 +7860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>16</v>
       </c>
@@ -7870,7 +7886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>16</v>
       </c>
@@ -7896,7 +7912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -7922,7 +7938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>16</v>
       </c>
@@ -7948,7 +7964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>16</v>
       </c>
@@ -7974,7 +7990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>16</v>
       </c>
@@ -8000,7 +8016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>16</v>
       </c>
@@ -8026,7 +8042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>16</v>
       </c>
@@ -8052,7 +8068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>16</v>
       </c>
@@ -8078,7 +8094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>16</v>
       </c>
@@ -8104,7 +8120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>16</v>
       </c>
@@ -8130,7 +8146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -8156,7 +8172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>16</v>
       </c>
@@ -8182,7 +8198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>16</v>
       </c>
@@ -8208,7 +8224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>16</v>
       </c>
@@ -8234,7 +8250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>16</v>
       </c>
@@ -8260,7 +8276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>16</v>
       </c>
@@ -8286,7 +8302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>16</v>
       </c>
@@ -8312,7 +8328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>16</v>
       </c>
@@ -8338,7 +8354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>16</v>
       </c>
@@ -8364,7 +8380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>16</v>
       </c>
@@ -8390,7 +8406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>16</v>
       </c>
@@ -8416,7 +8432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>16</v>
       </c>
@@ -8442,7 +8458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>16</v>
       </c>
@@ -8468,7 +8484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>16</v>
       </c>
@@ -8494,7 +8510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>16</v>
       </c>
@@ -8520,7 +8536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>16</v>
       </c>
@@ -8546,7 +8562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>16</v>
       </c>
@@ -8572,7 +8588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>16</v>
       </c>
@@ -8598,7 +8614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>16</v>
       </c>
@@ -8624,7 +8640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>16</v>
       </c>
@@ -8650,7 +8666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>16</v>
       </c>
@@ -8676,7 +8692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>16</v>
       </c>
@@ -8702,7 +8718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>16</v>
       </c>
@@ -8728,7 +8744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>16</v>
       </c>
@@ -8754,7 +8770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>16</v>
       </c>
@@ -8780,7 +8796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>16</v>
       </c>
@@ -8806,7 +8822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>16</v>
       </c>
@@ -8832,7 +8848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>16</v>
       </c>
@@ -8858,7 +8874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>16</v>
       </c>
@@ -8884,7 +8900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>16</v>
       </c>
@@ -8910,7 +8926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>16</v>
       </c>
@@ -8936,7 +8952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>16</v>
       </c>
@@ -8962,7 +8978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>16</v>
       </c>
@@ -8988,7 +9004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>16</v>
       </c>
@@ -9014,7 +9030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>16</v>
       </c>
@@ -9040,7 +9056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>16</v>
       </c>
@@ -9066,7 +9082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>16</v>
       </c>
@@ -9092,7 +9108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>16</v>
       </c>
@@ -9118,7 +9134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>16</v>
       </c>
@@ -9144,7 +9160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>16</v>
       </c>
@@ -9170,7 +9186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>16</v>
       </c>
@@ -9196,7 +9212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>16</v>
       </c>
@@ -9222,7 +9238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>16</v>
       </c>
@@ -9248,7 +9264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>16</v>
       </c>
@@ -9274,7 +9290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>16</v>
       </c>
@@ -9300,7 +9316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>16</v>
       </c>
@@ -9326,7 +9342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>16</v>
       </c>
@@ -9352,7 +9368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>16</v>
       </c>
@@ -9378,7 +9394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>16</v>
       </c>
@@ -9404,7 +9420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>16</v>
       </c>
@@ -9430,7 +9446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>16</v>
       </c>
@@ -9456,7 +9472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>16</v>
       </c>
@@ -9482,7 +9498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>16</v>
       </c>
@@ -9508,7 +9524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>16</v>
       </c>
@@ -9534,7 +9550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>16</v>
       </c>
@@ -9560,7 +9576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>16</v>
       </c>
@@ -9586,7 +9602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>16</v>
       </c>
@@ -9612,7 +9628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>16</v>
       </c>
@@ -9638,7 +9654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>16</v>
       </c>
@@ -9665,10 +9681,20 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H119">
+  <autoFilter ref="A1:H119" xr:uid="{00000000-0009-0000-0000-000003000000}">
     <filterColumn colId="6">
       <filters>
-        <filter val="1"/>
+        <filter val="0.8701"/>
+        <filter val="0.8805"/>
+        <filter val="0.9158"/>
+        <filter val="0.9176"/>
+        <filter val="0.9238"/>
+        <filter val="0.9263"/>
+        <filter val="0.9279"/>
+        <filter val="0.9525"/>
+        <filter val="0.9544"/>
+        <filter val="0.9691"/>
+        <filter val="0.9697"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -9677,7 +9703,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>